<commit_message>
adding a plot for observed ice-off dates over time
</commit_message>
<xml_diff>
--- a/Input_Files/ice_off_dates20240918.xlsx
+++ b/Input_Files/ice_off_dates20240918.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gagers/Documents/Loch Vale &amp; Oleksy/Ice Phenology Project/Ice_Pheno/Input_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gagers/Documents/Thesis and Lab/Ice Phenology Project/Ice_Pheno/Input_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3406CF63-3358-1A46-AB92-A2F862E3B6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E791B7-B0D3-D242-B378-50FD8A2DABC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="740" windowWidth="19720" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>wy_doy_ice_off</t>
+  </si>
+  <si>
+    <t>waterYear</t>
   </si>
 </sst>
 </file>
@@ -424,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -435,100 +438,136 @@
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>41429</v>
       </c>
       <c r="B2">
         <v>247</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>41793</v>
       </c>
       <c r="B3">
         <v>246</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>42150</v>
       </c>
       <c r="B4">
         <v>238</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>42528</v>
       </c>
       <c r="B5">
         <v>250</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>42885</v>
       </c>
       <c r="B6">
         <v>242</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43242</v>
       </c>
       <c r="B7">
         <v>234</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43632</v>
       </c>
       <c r="B8">
         <v>259</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43973</v>
       </c>
       <c r="B9">
         <v>234</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>44358</v>
       </c>
       <c r="B10">
         <v>254</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>44712</v>
       </c>
       <c r="B11">
         <v>243</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45076</v>
       </c>
       <c r="B12">
         <v>242</v>
+      </c>
+      <c r="C12">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding WY 2024 data and figures, also using met data from Charlie
</commit_message>
<xml_diff>
--- a/Input_Files/ice_off_dates20240918.xlsx
+++ b/Input_Files/ice_off_dates20240918.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gagers/Documents/Thesis and Lab/Ice Phenology Project/Ice_Pheno/Input_Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E791B7-B0D3-D242-B378-50FD8A2DABC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23A206A7-20F8-ED4D-BD5B-3A8EB705BF9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="740" windowWidth="19720" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8140" yWindow="1600" windowWidth="19720" windowHeight="13180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,10 +89,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -570,6 +571,28 @@
         <v>2023</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>45449</v>
+      </c>
+      <c r="B13">
+        <v>250</v>
+      </c>
+      <c r="C13">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>45783</v>
+      </c>
+      <c r="B14">
+        <v>218</v>
+      </c>
+      <c r="C14">
+        <v>2025</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>